<commit_message>
Working on user management and dashboard.
</commit_message>
<xml_diff>
--- a/changes.xlsx
+++ b/changes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>groups table -&gt;column name "group_name" to name</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Change the DB Table "Final Review"</t>
+  </si>
+  <si>
+    <t>Change the DB Table "Dissemination_reviews"</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,6 +441,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working for approval section
</commit_message>
<xml_diff>
--- a/changes.xlsx
+++ b/changes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>groups table -&gt;column name "group_name" to name</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Change the DB Table "Dissemination_reviews"</t>
+  </si>
+  <si>
+    <t>Add new table Level of permission</t>
   </si>
 </sst>
 </file>
@@ -59,12 +62,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,14 +446,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>